<commit_message>
Se crea la clase tipo tarea CargarEprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBACCDD-DDF6-4876-BCBD-47662BE98F12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E425FBA-10A9-4C75-8D28-FA8B74C6A863}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>ACTIVO</t>
+  </si>
+  <si>
+    <t>valorRecarga</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -154,11 +157,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -168,6 +182,8 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -462,7 +478,7 @@
     <col min="5" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
+    <row r="1" spans="1:13" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,8 +515,11 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="15.5">
+    <row r="2" spans="1:13" ht="15.5">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -536,6 +555,9 @@
       </c>
       <c r="L2" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="M2" s="6">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactorización de la clase solictudEprepago - SolicitarEprepago, se refactorizaron las clases SolicitarEprepagoPage con su respectivo Locator, se refactoriza la tarea solicitarEprepago y se agrega un scroll
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E425FBA-10A9-4C75-8D28-FA8B74C6A863}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDF6BE9-2910-4E76-8928-35D1DFEA5ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>validarClave</t>
   </si>
   <si>
-    <t>autotest27</t>
-  </si>
-  <si>
     <t>Acierto</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>valorRecarga</t>
+  </si>
+  <si>
+    <t>testing10</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -516,7 +516,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.5">
@@ -524,13 +524,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>93221451</v>
+        <v>48313974</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3">
         <v>1234</v>
@@ -539,22 +539,22 @@
         <v>4321</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="M2" s="6">
         <v>10000</v>

</xml_diff>

<commit_message>
Se crea el Scenario recarga ePrepago sobre el valor maximo, se crea la tarea CargarValor, se crea la clase question ValorRecarga y la clase exception NoSeRealizoRecargaEprepagoException
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2083AB66-6189-45FD-A16F-3CDB57A07856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CD3571-7213-4D4A-93C4-F02AA2708B1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
+    <sheet name="CargaSobreMaximo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -103,6 +104,9 @@
   </si>
   <si>
     <t>406-739740-05</t>
+  </si>
+  <si>
+    <t>autotest25</t>
   </si>
 </sst>
 </file>
@@ -482,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -596,8 +600,70 @@
         <v>25</v>
       </c>
     </row>
+    <row r="3" spans="1:16" ht="15.5">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>93221450</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1234</v>
+      </c>
+      <c r="F3" s="3">
+        <v>4321</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="6">
+        <v>3000000</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5B451D-3C7E-405C-B9AB-67862CCEB21F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor a tarea de cargue
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/e-prepago/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CD3571-7213-4D4A-93C4-F02AA2708B1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
     <sheet name="CargaSobreMaximo" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -83,12 +85,6 @@
   </si>
   <si>
     <t>valorRecarga</t>
-  </si>
-  <si>
-    <t>opcionSubmenu</t>
-  </si>
-  <si>
-    <t>Recargar</t>
   </si>
   <si>
     <t>autotest27</t>
@@ -112,8 +108,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,22 +481,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,16 +537,13 @@
         <v>18</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.5">
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -561,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3">
         <v>1234</v>
@@ -591,16 +584,13 @@
         <v>10000</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.5">
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -611,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3">
         <v>1234</v>
@@ -641,13 +631,10 @@
         <v>3000000</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -657,12 +644,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5B451D-3C7E-405C-B9AB-67862CCEB21F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se refactoriza la tarea DescargarSaldo
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4B5362-5797-43C5-97C0-90E2803F26A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55602ECB-D246-47A8-A6CC-82F952DCD4F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,13 +103,13 @@
     <t>autotest25</t>
   </si>
   <si>
-    <t>autotest32</t>
-  </si>
-  <si>
     <t>406-733040-20</t>
   </si>
   <si>
     <t>10000</t>
+  </si>
+  <si>
+    <t>autotest26</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
@@ -555,13 +555,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>333333304</v>
+        <v>93221451</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3">
         <v>1234</v>
@@ -588,13 +588,13 @@
         <v>17</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.5">

</xml_diff>

<commit_message>
Estabilizacion de transacción de carga de eprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/e-prepago/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBB953A-A841-4A2F-923F-2581ABDB992D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -18,11 +17,11 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -103,22 +102,29 @@
     <t>autotest25</t>
   </si>
   <si>
-    <t>1000000</t>
-  </si>
-  <si>
-    <t>autotest32</t>
-  </si>
-  <si>
-    <t>406-733040-20</t>
+    <t>autotest30</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>406-733020-15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -197,18 +203,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,22 +497,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" zoomScalePageLayoutView="108" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +559,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.5">
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -560,8 +569,8 @@
       <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
+      <c r="D2" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="E2" s="3">
         <v>1234</v>
@@ -588,16 +597,16 @@
         <v>17</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.5">
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -651,12 +660,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mapeo de descarga de eprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/cargar_tarjeta_virtual_eprepago.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -109,15 +109,28 @@
   </si>
   <si>
     <t>406-733020-15</t>
+  </si>
+  <si>
+    <t>autotest28</t>
+  </si>
+  <si>
+    <t>406-714530-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -203,18 +216,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -498,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" zoomScalePageLayoutView="108" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -608,7 +624,7 @@
     </row>
     <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>93221450</v>
@@ -643,14 +659,61 @@
       <c r="L3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="6">
-        <v>3000000</v>
+      <c r="M3" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>93221453</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1234</v>
+      </c>
+      <c r="F4" s="3">
+        <v>4321</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>